<commit_message>
Updated Statistical Analysis Files
Modified Spreadsheet to include full descriptive statistics. Modified MiniTab Document to re-order data from Small to Large
</commit_message>
<xml_diff>
--- a/Statistical Analysis/Stastical Study of Seed Properties.xlsx
+++ b/Statistical Analysis/Stastical Study of Seed Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shash\Documents\GitHub\samaraAnalysis\Statistical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D852C-1942-428A-B6D0-3706D740CBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A21792-1270-4474-B32A-1061D0F9AF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{70F3C3AB-0120-463F-BA39-B2976DA3DFB9}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="Transition Time Stats MASTER" sheetId="8" r:id="rId3"/>
     <sheet name="Rounded Properties" sheetId="9" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">sampleProperties_revA!$C$3:$C$102</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">sampleProperties_revA!$F$3:$F$102</definedName>
@@ -46,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="68">
   <si>
     <t>Explanatory Variables</t>
   </si>
@@ -241,6 +238,15 @@
   </si>
   <si>
     <t>Aspect Ratio = b^2/A Rounded</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Span</t>
+  </si>
+  <si>
+    <t>Chord</t>
   </si>
 </sst>
 </file>
@@ -787,7 +793,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="8" xfId="15" applyFont="1"/>
@@ -849,9 +855,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -899,10 +902,6 @@
   </cellStyles>
   <dxfs count="90">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -916,6 +915,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1004,7 +1007,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1016,11 +1031,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1047,35 +1079,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4617,16 +4620,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>2254250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>911225</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -4662,7 +4665,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="20608925" y="3330575"/>
+              <a:off x="26695400" y="3844925"/>
               <a:ext cx="7251700" cy="3702050"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4823,8 +4826,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="54257576" y="876300"/>
-              <a:ext cx="10321925" cy="1819275"/>
+              <a:off x="54257576" y="5734050"/>
+              <a:ext cx="10321925" cy="11439525"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4906,8 +4909,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="54257576" y="876300"/>
-              <a:ext cx="10321925" cy="1819275"/>
+              <a:off x="54038501" y="6000750"/>
+              <a:ext cx="10321925" cy="11439525"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4989,8 +4992,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="54038501" y="6000750"/>
-              <a:ext cx="10321925" cy="11439525"/>
+              <a:off x="52800251" y="5991225"/>
+              <a:ext cx="10321925" cy="11430000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5021,2371 +5024,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="2 Sample T Test Loading Differe"/>
-      <sheetName val="2 Sample T Test Mass Difference"/>
-      <sheetName val="2 Sample T Test  Span, Chord, A"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="K2" t="str">
-            <v>Mass Count</v>
-          </cell>
-          <cell r="L2" t="str">
-            <v>Span</v>
-          </cell>
-          <cell r="M2" t="str">
-            <v>Chord</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="J3" t="str">
-            <v>S</v>
-          </cell>
-          <cell r="K3">
-            <v>16</v>
-          </cell>
-          <cell r="L3">
-            <v>28</v>
-          </cell>
-          <cell r="M3">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="J4" t="str">
-            <v>M</v>
-          </cell>
-          <cell r="K4">
-            <v>47</v>
-          </cell>
-          <cell r="L4">
-            <v>28</v>
-          </cell>
-          <cell r="M4">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5" t="str">
-            <v>L</v>
-          </cell>
-          <cell r="K5">
-            <v>20</v>
-          </cell>
-          <cell r="L5">
-            <v>27</v>
-          </cell>
-          <cell r="M5">
-            <v>27</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="F2" t="str">
-            <v>t = 𝑓(L)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3">
-            <v>1.3610558365817524</v>
-          </cell>
-          <cell r="E3">
-            <v>0.43</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>2.2291257182786146</v>
-          </cell>
-          <cell r="E4">
-            <v>0.46899999999999997</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>2.4437219585871164</v>
-          </cell>
-          <cell r="E5">
-            <v>0.42199999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>2.6746962496154434</v>
-          </cell>
-          <cell r="E6">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>2.7364260203259771</v>
-          </cell>
-          <cell r="E7">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>2.8918759706528143</v>
-          </cell>
-          <cell r="E8">
-            <v>0.44750000000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>2.954511492356906</v>
-          </cell>
-          <cell r="E9">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>3.0362354200472272</v>
-          </cell>
-          <cell r="E10">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>3.0401773019832694</v>
-          </cell>
-          <cell r="E11">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>3.0437996971166115</v>
-          </cell>
-          <cell r="E12">
-            <v>0.436</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>3.0540548639419152</v>
-          </cell>
-          <cell r="E13">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>3.168022413121093</v>
-          </cell>
-          <cell r="E14">
-            <v>0.55300000000000005</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>3.1689513053664067</v>
-          </cell>
-          <cell r="E15">
-            <v>0.45200000000000001</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>3.2004053194259794</v>
-          </cell>
-          <cell r="E16">
-            <v>0.433</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>3.2072543293491194</v>
-          </cell>
-          <cell r="E17">
-            <v>0.439</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>3.2708114419822603</v>
-          </cell>
-          <cell r="E18">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>3.3274551574824494</v>
-          </cell>
-          <cell r="E19">
-            <v>0.53900000000000003</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>3.3575719222709162</v>
-          </cell>
-          <cell r="E20">
-            <v>0.375</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="D21">
-            <v>3.3962241725007543</v>
-          </cell>
-          <cell r="E21">
-            <v>0.44500000000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="D22">
-            <v>3.4269775052524092</v>
-          </cell>
-          <cell r="E22">
-            <v>0.45800000000000002</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
-            <v>3.5356369789885709</v>
-          </cell>
-          <cell r="E23">
-            <v>0.49299999999999999</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24">
-            <v>3.5995643166607585</v>
-          </cell>
-          <cell r="E24">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="D25">
-            <v>3.7025797561023834</v>
-          </cell>
-          <cell r="E25">
-            <v>0.44900000000000001</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="D26">
-            <v>3.7377439219630704</v>
-          </cell>
-          <cell r="E26">
-            <v>0.51800000000000002</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="D27">
-            <v>3.7492139835943572</v>
-          </cell>
-          <cell r="E27">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="D28">
-            <v>3.7870082748972034</v>
-          </cell>
-          <cell r="E28">
-            <v>0.50600000000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="D29">
-            <v>3.789153020747706</v>
-          </cell>
-          <cell r="E29">
-            <v>0.45300000000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="D30">
-            <v>3.8286475655613081</v>
-          </cell>
-          <cell r="E30">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="D31">
-            <v>3.9007959475716447</v>
-          </cell>
-          <cell r="E31">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="D32">
-            <v>3.9280324867266141</v>
-          </cell>
-          <cell r="E32">
-            <v>0.48499999999999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="D33">
-            <v>3.9439100073669562</v>
-          </cell>
-          <cell r="E33">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="D34">
-            <v>3.9696500546698918</v>
-          </cell>
-          <cell r="E34">
-            <v>0.53</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="D35">
-            <v>3.9930880390931285</v>
-          </cell>
-          <cell r="E35">
-            <v>0.443</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="D36">
-            <v>4.0110421873456508</v>
-          </cell>
-          <cell r="E36">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="D37">
-            <v>4.012502683499215</v>
-          </cell>
-          <cell r="E37">
-            <v>0.621</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="D38">
-            <v>4.066769246830658</v>
-          </cell>
-          <cell r="E38">
-            <v>0.379</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="D39">
-            <v>4.0961129410557149</v>
-          </cell>
-          <cell r="E39">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="D40">
-            <v>4.1281561340760096</v>
-          </cell>
-          <cell r="E40">
-            <v>0.55700000000000005</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="D41">
-            <v>4.1328919274434623</v>
-          </cell>
-          <cell r="E41">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="D42">
-            <v>4.1354464758581209</v>
-          </cell>
-          <cell r="E42">
-            <v>0.52700000000000002</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="D43">
-            <v>4.1644968300958123</v>
-          </cell>
-          <cell r="E43">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="D44">
-            <v>4.1935826776435272</v>
-          </cell>
-          <cell r="E44">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="D45">
-            <v>4.2038086330521107</v>
-          </cell>
-          <cell r="E45">
-            <v>0.45700000000000002</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="D46">
-            <v>4.255695714365749</v>
-          </cell>
-          <cell r="E46">
-            <v>0.51</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="D47">
-            <v>4.2829383934042768</v>
-          </cell>
-          <cell r="E47">
-            <v>0.51100000000000001</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="D48">
-            <v>4.3431775587797716</v>
-          </cell>
-          <cell r="E48">
-            <v>0.47299999999999998</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="D49">
-            <v>4.406862511311302</v>
-          </cell>
-          <cell r="E49">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="D50">
-            <v>4.4157959009735821</v>
-          </cell>
-          <cell r="E50">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="D51">
-            <v>4.4212150789617173</v>
-          </cell>
-          <cell r="E51">
-            <v>0.54100000000000004</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="D52">
-            <v>4.4241386093215374</v>
-          </cell>
-          <cell r="E52">
-            <v>0.40600000000000003</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="D53">
-            <v>4.4606778618607805</v>
-          </cell>
-          <cell r="E53">
-            <v>0.52900000000000003</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="D54">
-            <v>4.5106357853698462</v>
-          </cell>
-          <cell r="E54">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="D55">
-            <v>4.5501390617117901</v>
-          </cell>
-          <cell r="E55">
-            <v>0.48299999999999998</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="D56">
-            <v>4.5797757086498967</v>
-          </cell>
-          <cell r="E56">
-            <v>0.501</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="D57">
-            <v>4.6450712955373179</v>
-          </cell>
-          <cell r="E57">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="D58">
-            <v>4.6502600313952644</v>
-          </cell>
-          <cell r="E58">
-            <v>0.46800000000000003</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="D59">
-            <v>4.670782023987357</v>
-          </cell>
-          <cell r="E59">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="D60">
-            <v>4.6717138492640053</v>
-          </cell>
-          <cell r="E60">
-            <v>0.39800000000000002</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="D61">
-            <v>4.7063365244340707</v>
-          </cell>
-          <cell r="E61">
-            <v>0.36399999999999999</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="D62">
-            <v>4.7724794181372339</v>
-          </cell>
-          <cell r="E62">
-            <v>0.51400000000000001</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="D63">
-            <v>4.7942604058611771</v>
-          </cell>
-          <cell r="E63">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="D64">
-            <v>4.8121172703560564</v>
-          </cell>
-          <cell r="E64">
-            <v>0.51900000000000002</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="D65">
-            <v>4.8574518248908021</v>
-          </cell>
-          <cell r="E65">
-            <v>0.47099999999999997</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="D66">
-            <v>4.8861691536095515</v>
-          </cell>
-          <cell r="E66">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="D67">
-            <v>4.894467024369427</v>
-          </cell>
-          <cell r="E67">
-            <v>0.376</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="D68">
-            <v>4.9704358016183088</v>
-          </cell>
-          <cell r="E68">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="D69">
-            <v>5.0052293830451111</v>
-          </cell>
-          <cell r="E69">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="D70">
-            <v>5.0372606982584704</v>
-          </cell>
-          <cell r="E70">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="D71">
-            <v>5.1110146951484667</v>
-          </cell>
-          <cell r="E71">
-            <v>0.438</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="D72">
-            <v>5.1874393198602542</v>
-          </cell>
-          <cell r="E72">
-            <v>0.42499999999999999</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="D73">
-            <v>5.2634222676918059</v>
-          </cell>
-          <cell r="E73">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="D74">
-            <v>5.6392451946761533</v>
-          </cell>
-          <cell r="E74">
-            <v>0.48399999999999999</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="D75">
-            <v>5.6747766069205259</v>
-          </cell>
-          <cell r="E75">
-            <v>0.55000000000000004</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="D76">
-            <v>5.7648856890442497</v>
-          </cell>
-          <cell r="E76">
-            <v>0.42</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="D77">
-            <v>5.848393024064273</v>
-          </cell>
-          <cell r="E77">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="D78">
-            <v>5.8725932689034357</v>
-          </cell>
-          <cell r="E78">
-            <v>0.44</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="D79">
-            <v>5.9509442614804868</v>
-          </cell>
-          <cell r="E79">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="D80">
-            <v>5.9661059028449284</v>
-          </cell>
-          <cell r="E80">
-            <v>0.45600000000000002</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="D81">
-            <v>6.0403043623078121</v>
-          </cell>
-          <cell r="E81">
-            <v>0.51300000000000001</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="D82">
-            <v>6.2542530169027897</v>
-          </cell>
-          <cell r="E82">
-            <v>0.624</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="D83">
-            <v>7.2404944095118591</v>
-          </cell>
-          <cell r="E83">
-            <v>0.47499999999999998</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="D84">
-            <v>7.2836596199072723</v>
-          </cell>
-          <cell r="E84">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="D85">
-            <v>7.3267967228701929</v>
-          </cell>
-          <cell r="E85">
-            <v>0.60399999999999998</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="D86">
-            <v>7.5547302540519432</v>
-          </cell>
-          <cell r="E86">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="F2" t="str">
-            <v>t = 𝑓(m)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3">
-            <v>0.4</v>
-          </cell>
-          <cell r="E3">
-            <v>0.36399999999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>0.4</v>
-          </cell>
-          <cell r="E4">
-            <v>0.375</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>0.4</v>
-          </cell>
-          <cell r="E5">
-            <v>0.376</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>0.4</v>
-          </cell>
-          <cell r="E6">
-            <v>0.379</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>0.3</v>
-          </cell>
-          <cell r="E7">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>0.5</v>
-          </cell>
-          <cell r="E8">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>0.3</v>
-          </cell>
-          <cell r="E9">
-            <v>0.39800000000000002</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>0.5</v>
-          </cell>
-          <cell r="E10">
-            <v>0.40600000000000003</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>0.3</v>
-          </cell>
-          <cell r="E11">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>0.3</v>
-          </cell>
-          <cell r="E12">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>0.5</v>
-          </cell>
-          <cell r="E13">
-            <v>0.42</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>0.2</v>
-          </cell>
-          <cell r="E14">
-            <v>0.42199999999999999</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>0.6</v>
-          </cell>
-          <cell r="E15">
-            <v>0.42499999999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>0.1</v>
-          </cell>
-          <cell r="E16">
-            <v>0.43</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>0.4</v>
-          </cell>
-          <cell r="E17">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>0.6</v>
-          </cell>
-          <cell r="E18">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>0.4</v>
-          </cell>
-          <cell r="E19">
-            <v>0.433</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>0.3</v>
-          </cell>
-          <cell r="E20">
-            <v>0.436</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="D21">
-            <v>0.6</v>
-          </cell>
-          <cell r="E21">
-            <v>0.438</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="D22">
-            <v>0.4</v>
-          </cell>
-          <cell r="E22">
-            <v>0.439</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
-            <v>0.6</v>
-          </cell>
-          <cell r="E23">
-            <v>0.44</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24">
-            <v>0.5</v>
-          </cell>
-          <cell r="E24">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="D25">
-            <v>0.5</v>
-          </cell>
-          <cell r="E25">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="D26">
-            <v>0.4</v>
-          </cell>
-          <cell r="E26">
-            <v>0.443</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="D27">
-            <v>0.3</v>
-          </cell>
-          <cell r="E27">
-            <v>0.44500000000000001</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="D28">
-            <v>0.3</v>
-          </cell>
-          <cell r="E28">
-            <v>0.44750000000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="D29">
-            <v>0.5</v>
-          </cell>
-          <cell r="E29">
-            <v>0.44900000000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="D30">
-            <v>0.5</v>
-          </cell>
-          <cell r="E30">
-            <v>0.45200000000000001</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="D31">
-            <v>0.3</v>
-          </cell>
-          <cell r="E31">
-            <v>0.45300000000000001</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="D32">
-            <v>0.6</v>
-          </cell>
-          <cell r="E32">
-            <v>0.45600000000000002</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="D33">
-            <v>0.6</v>
-          </cell>
-          <cell r="E33">
-            <v>0.45700000000000002</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="D34">
-            <v>0.4</v>
-          </cell>
-          <cell r="E34">
-            <v>0.45800000000000002</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="D35">
-            <v>0.4</v>
-          </cell>
-          <cell r="E35">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="D36">
-            <v>0.4</v>
-          </cell>
-          <cell r="E36">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="D37">
-            <v>0.3</v>
-          </cell>
-          <cell r="E37">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="D38">
-            <v>0.5</v>
-          </cell>
-          <cell r="E38">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="D39">
-            <v>0.8</v>
-          </cell>
-          <cell r="E39">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="D40">
-            <v>0.5</v>
-          </cell>
-          <cell r="E40">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="D41">
-            <v>0.6</v>
-          </cell>
-          <cell r="E41">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="D42">
-            <v>0.4</v>
-          </cell>
-          <cell r="E42">
-            <v>0.46800000000000003</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="D43">
-            <v>0.2</v>
-          </cell>
-          <cell r="E43">
-            <v>0.46899999999999997</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="D44">
-            <v>0.3</v>
-          </cell>
-          <cell r="E44">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="D45">
-            <v>0.4</v>
-          </cell>
-          <cell r="E45">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="D46">
-            <v>0.5</v>
-          </cell>
-          <cell r="E46">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="D47">
-            <v>0.6</v>
-          </cell>
-          <cell r="E47">
-            <v>0.47099999999999997</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="D48">
-            <v>0.3</v>
-          </cell>
-          <cell r="E48">
-            <v>0.47299999999999998</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="D49">
-            <v>0.5</v>
-          </cell>
-          <cell r="E49">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="D50">
-            <v>0.5</v>
-          </cell>
-          <cell r="E50">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="D51">
-            <v>0.6</v>
-          </cell>
-          <cell r="E51">
-            <v>0.47499999999999998</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="D52">
-            <v>0.4</v>
-          </cell>
-          <cell r="E52">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="D53">
-            <v>0.5</v>
-          </cell>
-          <cell r="E53">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="D54">
-            <v>0.6</v>
-          </cell>
-          <cell r="E54">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="D55">
-            <v>0.4</v>
-          </cell>
-          <cell r="E55">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="D56">
-            <v>0.4</v>
-          </cell>
-          <cell r="E56">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="D57">
-            <v>0.4</v>
-          </cell>
-          <cell r="E57">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="D58">
-            <v>0.7</v>
-          </cell>
-          <cell r="E58">
-            <v>0.48299999999999998</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="D59">
-            <v>0.6</v>
-          </cell>
-          <cell r="E59">
-            <v>0.48399999999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="D60">
-            <v>0.5</v>
-          </cell>
-          <cell r="E60">
-            <v>0.48499999999999999</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="D61">
-            <v>0.4</v>
-          </cell>
-          <cell r="E61">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="D62">
-            <v>0.5</v>
-          </cell>
-          <cell r="E62">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="D63">
-            <v>0.4</v>
-          </cell>
-          <cell r="E63">
-            <v>0.49299999999999999</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="D64">
-            <v>0.5</v>
-          </cell>
-          <cell r="E64">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="D65">
-            <v>0.4</v>
-          </cell>
-          <cell r="E65">
-            <v>0.501</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="D66">
-            <v>0.5</v>
-          </cell>
-          <cell r="E66">
-            <v>0.50600000000000001</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="D67">
-            <v>0.4</v>
-          </cell>
-          <cell r="E67">
-            <v>0.51</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="D68">
-            <v>0.6</v>
-          </cell>
-          <cell r="E68">
-            <v>0.51100000000000001</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="D69">
-            <v>0.7</v>
-          </cell>
-          <cell r="E69">
-            <v>0.51300000000000001</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="D70">
-            <v>0.6</v>
-          </cell>
-          <cell r="E70">
-            <v>0.51400000000000001</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="D71">
-            <v>0.4</v>
-          </cell>
-          <cell r="E71">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="D72">
-            <v>0.4</v>
-          </cell>
-          <cell r="E72">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="D73">
-            <v>0.7</v>
-          </cell>
-          <cell r="E73">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="D74">
-            <v>0.4</v>
-          </cell>
-          <cell r="E74">
-            <v>0.51800000000000002</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="D75">
-            <v>0.6</v>
-          </cell>
-          <cell r="E75">
-            <v>0.51900000000000002</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="D76">
-            <v>0.4</v>
-          </cell>
-          <cell r="E76">
-            <v>0.52700000000000002</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="D77">
-            <v>0.7</v>
-          </cell>
-          <cell r="E77">
-            <v>0.52900000000000003</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="D78">
-            <v>0.5</v>
-          </cell>
-          <cell r="E78">
-            <v>0.53</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="D79">
-            <v>0.3</v>
-          </cell>
-          <cell r="E79">
-            <v>0.53900000000000003</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="D80">
-            <v>0.5</v>
-          </cell>
-          <cell r="E80">
-            <v>0.54100000000000004</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="D81">
-            <v>0.5</v>
-          </cell>
-          <cell r="E81">
-            <v>0.55000000000000004</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="D82">
-            <v>0.3</v>
-          </cell>
-          <cell r="E82">
-            <v>0.55300000000000005</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="D83">
-            <v>0.4</v>
-          </cell>
-          <cell r="E83">
-            <v>0.55700000000000005</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="D84">
-            <v>0.7</v>
-          </cell>
-          <cell r="E84">
-            <v>0.60399999999999998</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="D85">
-            <v>0.5</v>
-          </cell>
-          <cell r="E85">
-            <v>0.621</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="D86">
-            <v>0.6</v>
-          </cell>
-          <cell r="E86">
-            <v>0.624</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="L2" t="str">
-            <v>t = 𝑓(b)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>45.104956880000003</v>
-          </cell>
-          <cell r="D3">
-            <v>19.41453533</v>
-          </cell>
-          <cell r="F3">
-            <v>0.39800000000000002</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>50.02547852</v>
-          </cell>
-          <cell r="D4">
-            <v>17.710400230000001</v>
-          </cell>
-          <cell r="F4">
-            <v>0.47299999999999998</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>48.301828579999999</v>
-          </cell>
-          <cell r="D5">
-            <v>19.806350930000001</v>
-          </cell>
-          <cell r="F5">
-            <v>0.43</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>52.039158950000001</v>
-          </cell>
-          <cell r="D6">
-            <v>19.519087580000001</v>
-          </cell>
-          <cell r="F6">
-            <v>0.45300000000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>53.450201389999997</v>
-          </cell>
-          <cell r="D7">
-            <v>19.20213996</v>
-          </cell>
-          <cell r="F7">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>52.21334693</v>
-          </cell>
-          <cell r="D8">
-            <v>20.84662719</v>
-          </cell>
-          <cell r="F8">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>55.336607649999998</v>
-          </cell>
-          <cell r="D9">
-            <v>19.269757519999999</v>
-          </cell>
-          <cell r="F9">
-            <v>0.376</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>51.683831099999999</v>
-          </cell>
-          <cell r="D10">
-            <v>20.009116330000001</v>
-          </cell>
-          <cell r="F10">
-            <v>0.42199999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>53.709470430000003</v>
-          </cell>
-          <cell r="D11">
-            <v>20.494740360000002</v>
-          </cell>
-          <cell r="F11">
-            <v>0.47499999999999998</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>52.423031039999998</v>
-          </cell>
-          <cell r="D12">
-            <v>21.229999979999999</v>
-          </cell>
-          <cell r="F12">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>51.887492109999997</v>
-          </cell>
-          <cell r="D13">
-            <v>22.175329519999998</v>
-          </cell>
-          <cell r="F13">
-            <v>0.36399999999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>49.967565999999998</v>
-          </cell>
-          <cell r="D14">
-            <v>22.285337470000002</v>
-          </cell>
-          <cell r="F14">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>53.642884649999999</v>
-          </cell>
-          <cell r="D15">
-            <v>21.331025650000001</v>
-          </cell>
-          <cell r="F15">
-            <v>0.46800000000000003</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>55.578320669999997</v>
-          </cell>
-          <cell r="D16">
-            <v>19.969545449999998</v>
-          </cell>
-          <cell r="F16">
-            <v>0.51700000000000002</v>
-          </cell>
-          <cell r="L16" t="str">
-            <v>t = 𝑓(c)</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>59.213153630000001</v>
-          </cell>
-          <cell r="D17">
-            <v>18.34600288</v>
-          </cell>
-          <cell r="F17">
-            <v>0.42</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>51.07267349</v>
-          </cell>
-          <cell r="D18">
-            <v>22.52203299</v>
-          </cell>
-          <cell r="F18">
-            <v>0.501</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>58.107452559999999</v>
-          </cell>
-          <cell r="D19">
-            <v>19.109597239999999</v>
-          </cell>
-          <cell r="F19">
-            <v>0.55000000000000004</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>56.060978550000002</v>
-          </cell>
-          <cell r="D20">
-            <v>20.0536052</v>
-          </cell>
-          <cell r="F20">
-            <v>0.44500000000000001</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>49.997458020000003</v>
-          </cell>
-          <cell r="D21">
-            <v>25.179504000000001</v>
-          </cell>
-          <cell r="F21">
-            <v>0.46899999999999997</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>55.28530482</v>
-          </cell>
-          <cell r="D22">
-            <v>20.518319479999999</v>
-          </cell>
-          <cell r="F22">
-            <v>0.53900000000000003</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>58.625620519999998</v>
-          </cell>
-          <cell r="D23">
-            <v>22.05077361</v>
-          </cell>
-          <cell r="F23">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>50.244893859999998</v>
-          </cell>
-          <cell r="D24">
-            <v>25.346974039999999</v>
-          </cell>
-          <cell r="F24">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>58.838548379999999</v>
-          </cell>
-          <cell r="D25">
-            <v>20.296107330000002</v>
-          </cell>
-          <cell r="F25">
-            <v>0.51</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>59.673597620000002</v>
-          </cell>
-          <cell r="D26">
-            <v>19.81942716</v>
-          </cell>
-          <cell r="F26">
-            <v>0.55300000000000005</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>56.294381440000002</v>
-          </cell>
-          <cell r="D27">
-            <v>21.16045677</v>
-          </cell>
-          <cell r="F27">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>65.606135850000001</v>
-          </cell>
-          <cell r="D28">
-            <v>19.610823719999999</v>
-          </cell>
-          <cell r="F28">
-            <v>0.60399999999999998</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>59.120296660000001</v>
-          </cell>
-          <cell r="D29">
-            <v>20.89870342</v>
-          </cell>
-          <cell r="F29">
-            <v>0.624</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>58.120535769999996</v>
-          </cell>
-          <cell r="D30">
-            <v>21.401459240000001</v>
-          </cell>
-          <cell r="F30">
-            <v>0.52700000000000002</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>57.590985019999998</v>
-          </cell>
-          <cell r="D31">
-            <v>21.9677212</v>
-          </cell>
-          <cell r="F31">
-            <v>0.55700000000000005</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>54.087389260000002</v>
-          </cell>
-          <cell r="D32">
-            <v>26.992702560000001</v>
-          </cell>
-          <cell r="F32">
-            <v>0.48799999999999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>55.399321190000002</v>
-          </cell>
-          <cell r="D33">
-            <v>24.702334990000001</v>
-          </cell>
-          <cell r="F33">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>51.313356470000002</v>
-          </cell>
-          <cell r="D34">
-            <v>26.100959379999999</v>
-          </cell>
-          <cell r="F34">
-            <v>0.379</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>58.901998650000003</v>
-          </cell>
-          <cell r="D35">
-            <v>21.888052200000001</v>
-          </cell>
-          <cell r="F35">
-            <v>0.436</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>57.330169179999999</v>
-          </cell>
-          <cell r="D36">
-            <v>22.241920539999999</v>
-          </cell>
-          <cell r="F36">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>61.022645799999999</v>
-          </cell>
-          <cell r="D37">
-            <v>20.37266352</v>
-          </cell>
-          <cell r="F37">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>62.70678771</v>
-          </cell>
-          <cell r="D38">
-            <v>20.03133545</v>
-          </cell>
-          <cell r="F38">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>62.928535480000001</v>
-          </cell>
-          <cell r="D39">
-            <v>20.780493580000002</v>
-          </cell>
-          <cell r="F39">
-            <v>0.443</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>61.48642083</v>
-          </cell>
-          <cell r="D40">
-            <v>21.171127250000001</v>
-          </cell>
-          <cell r="F40">
-            <v>0.45600000000000002</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>68.926039360000004</v>
-          </cell>
-          <cell r="D41">
-            <v>19.02712794</v>
-          </cell>
-          <cell r="F41">
-            <v>0.43099999999999999</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>63.05516368</v>
-          </cell>
-          <cell r="D42">
-            <v>20.824448220000001</v>
-          </cell>
-          <cell r="F42">
-            <v>0.45900000000000002</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>58.662226990000001</v>
-          </cell>
-          <cell r="D43">
-            <v>22.384278640000002</v>
-          </cell>
-          <cell r="F43">
-            <v>0.41</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>55.828151779999999</v>
-          </cell>
-          <cell r="D44">
-            <v>24.812590849999999</v>
-          </cell>
-          <cell r="F44">
-            <v>0.44</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>61.29023196</v>
-          </cell>
-          <cell r="D45">
-            <v>21.25493385</v>
-          </cell>
-          <cell r="F45">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>60.635882619999997</v>
-          </cell>
-          <cell r="D46">
-            <v>20.464591710000001</v>
-          </cell>
-          <cell r="F46">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>55.648433019999999</v>
-          </cell>
-          <cell r="D47">
-            <v>24.125772659999999</v>
-          </cell>
-          <cell r="F47">
-            <v>0.44750000000000001</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>59.979193889999998</v>
-          </cell>
-          <cell r="D48">
-            <v>22.958660439999999</v>
-          </cell>
-          <cell r="F48">
-            <v>0.48399999999999999</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>59.61057332</v>
-          </cell>
-          <cell r="D49">
-            <v>22.82143507</v>
-          </cell>
-          <cell r="F49">
-            <v>0.51800000000000002</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>61.968094059999999</v>
-          </cell>
-          <cell r="D50">
-            <v>21.986914800000001</v>
-          </cell>
-          <cell r="F50">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>60.648124350000003</v>
-          </cell>
-          <cell r="D51">
-            <v>22.247919199999998</v>
-          </cell>
-          <cell r="F51">
-            <v>0.38700000000000001</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>64.493521310000006</v>
-          </cell>
-          <cell r="D52">
-            <v>22.33357114</v>
-          </cell>
-          <cell r="F52">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>60.472124200000003</v>
-          </cell>
-          <cell r="D53">
-            <v>24.232992530000001</v>
-          </cell>
-          <cell r="F53">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>58.742765409999997</v>
-          </cell>
-          <cell r="D54">
-            <v>25.80899277</v>
-          </cell>
-          <cell r="F54">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>58.802109510000001</v>
-          </cell>
-          <cell r="D55">
-            <v>26.146429399999999</v>
-          </cell>
-          <cell r="F55">
-            <v>0.40600000000000003</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>63.453477239999998</v>
-          </cell>
-          <cell r="D56">
-            <v>22.894347719999999</v>
-          </cell>
-          <cell r="F56">
-            <v>0.54100000000000004</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>55.927126110000003</v>
-          </cell>
-          <cell r="D57">
-            <v>26.886526700000001</v>
-          </cell>
-          <cell r="F57">
-            <v>0.49299999999999999</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>61.567797249999998</v>
-          </cell>
-          <cell r="D58">
-            <v>25.140701279999998</v>
-          </cell>
-          <cell r="F58">
-            <v>0.47</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>64.170201430000006</v>
-          </cell>
-          <cell r="D59">
-            <v>22.907336659999999</v>
-          </cell>
-          <cell r="F59">
-            <v>0.42499999999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>62.894848029999999</v>
-          </cell>
-          <cell r="D60">
-            <v>23.827620589999999</v>
-          </cell>
-          <cell r="F60">
-            <v>0.51300000000000001</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>60.889320609999999</v>
-          </cell>
-          <cell r="D61">
-            <v>24.847767489999999</v>
-          </cell>
-          <cell r="F61">
-            <v>0.45800000000000002</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>64.825975349999993</v>
-          </cell>
-          <cell r="D62">
-            <v>23.395778459999999</v>
-          </cell>
-          <cell r="F62">
-            <v>0.438</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>61.121899470000002</v>
-          </cell>
-          <cell r="D63">
-            <v>24.832212179999999</v>
-          </cell>
-          <cell r="F63">
-            <v>0.375</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>61.626219550000002</v>
-          </cell>
-          <cell r="D64">
-            <v>24.346188349999998</v>
-          </cell>
-          <cell r="F64">
-            <v>0.442</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>60.992072909999997</v>
-          </cell>
-          <cell r="D65">
-            <v>25.908833040000001</v>
-          </cell>
-          <cell r="F65">
-            <v>0.47399999999999998</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>64.608019519999999</v>
-          </cell>
-          <cell r="D66">
-            <v>24.147801479999998</v>
-          </cell>
-          <cell r="F66">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>63.01222336</v>
-          </cell>
-          <cell r="D67">
-            <v>24.89640095</v>
-          </cell>
-          <cell r="F67">
-            <v>0.51700000000000002</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>63.843808889999998</v>
-          </cell>
-          <cell r="D68">
-            <v>25.913962269999999</v>
-          </cell>
-          <cell r="F68">
-            <v>0.47099999999999997</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>66.864931839999997</v>
-          </cell>
-          <cell r="D69">
-            <v>23.298256649999999</v>
-          </cell>
-          <cell r="F69">
-            <v>0.621</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>66.061817230000003</v>
-          </cell>
-          <cell r="D70">
-            <v>24.957359929999999</v>
-          </cell>
-          <cell r="F70">
-            <v>0.51900000000000002</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>63.866420820000002</v>
-          </cell>
-          <cell r="D71">
-            <v>26.152300610000001</v>
-          </cell>
-          <cell r="F71">
-            <v>0.439</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>65.456686210000001</v>
-          </cell>
-          <cell r="D72">
-            <v>24.3477788</v>
-          </cell>
-          <cell r="F72">
-            <v>0.433</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>72.835431290000002</v>
-          </cell>
-          <cell r="D73">
-            <v>22.428352</v>
-          </cell>
-          <cell r="F73">
-            <v>0.51400000000000001</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>67.751594670000003</v>
-          </cell>
-          <cell r="D74">
-            <v>23.318892309999999</v>
-          </cell>
-          <cell r="F74">
-            <v>0.53</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>64.350489330000002</v>
-          </cell>
-          <cell r="D75">
-            <v>25.62139685</v>
-          </cell>
-          <cell r="F75">
-            <v>0.48499999999999999</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>68.099411970000006</v>
-          </cell>
-          <cell r="D76">
-            <v>24.893639050000001</v>
-          </cell>
-          <cell r="F76">
-            <v>0.48</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>67.572598679999999</v>
-          </cell>
-          <cell r="D77">
-            <v>24.453595029999999</v>
-          </cell>
-          <cell r="F77">
-            <v>0.50600000000000001</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>63.371409479999997</v>
-          </cell>
-          <cell r="D78">
-            <v>26.830176689999998</v>
-          </cell>
-          <cell r="F78">
-            <v>0.44900000000000001</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>68.599611899999999</v>
-          </cell>
-          <cell r="D79">
-            <v>26.243106229999999</v>
-          </cell>
-          <cell r="F79">
-            <v>0.46300000000000002</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>69.816661719999999</v>
-          </cell>
-          <cell r="D80">
-            <v>25.269625250000001</v>
-          </cell>
-          <cell r="F80">
-            <v>0.51100000000000001</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>68.965620709999996</v>
-          </cell>
-          <cell r="D81">
-            <v>26.242538840000002</v>
-          </cell>
-          <cell r="F81">
-            <v>0.45700000000000002</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>67.947015379999996</v>
-          </cell>
-          <cell r="D82">
-            <v>29.286507660000002</v>
-          </cell>
-          <cell r="F82">
-            <v>0.48299999999999998</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>72.275133069999995</v>
-          </cell>
-          <cell r="D83">
-            <v>27.274993800000001</v>
-          </cell>
-          <cell r="F83">
-            <v>0.46600000000000003</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>69.936837359999998</v>
-          </cell>
-          <cell r="D84">
-            <v>29.294178809999998</v>
-          </cell>
-          <cell r="F84">
-            <v>0.52900000000000003</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>68.841331909999994</v>
-          </cell>
-          <cell r="D85">
-            <v>29.215817439999999</v>
-          </cell>
-          <cell r="F85">
-            <v>0.45200000000000001</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>72.912980860000005</v>
-          </cell>
-          <cell r="D86">
-            <v>27.675117780000001</v>
-          </cell>
-          <cell r="F86">
-            <v>0.47599999999999998</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7552,55 +5190,55 @@
     <tableColumn id="1" xr3:uid="{4F39DB47-9AEA-4CF9-91C2-8BF77F720469}" name="Num" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{E7D0B6C1-B0E5-472A-BEE1-85FDEE41A7FA}" name="id" dataDxfId="43"/>
     <tableColumn id="3" xr3:uid="{63134CDC-11EC-45EF-822F-F73E24FD15DB}" name="Mass [g]" dataDxfId="42" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="17" xr3:uid="{F33A7560-F44C-4419-9566-FC121DC9CF4A}" name="Mass [L,M,S]" dataDxfId="31" dataCellStyle="20% - Accent1">
+    <tableColumn id="17" xr3:uid="{F33A7560-F44C-4419-9566-FC121DC9CF4A}" name="Mass [L,M,S]" dataDxfId="41" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Mass '[g']]]&gt;0.5, "L", (IF(Table156[[#This Row],[Mass '[g']]]&gt;0.3, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BD5AEC8A-832A-407E-B092-B483D27F65EC}" name="Area [mm^2]" dataDxfId="32" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="5" xr3:uid="{80928843-3B8E-4E00-9BB2-3CB4E51EAAD3}" name="Area [mm^2] Rounded" dataDxfId="30" dataCellStyle="20% - Accent1">
+    <tableColumn id="4" xr3:uid="{BD5AEC8A-832A-407E-B092-B483D27F65EC}" name="Area [mm^2]" dataDxfId="40" dataCellStyle="20% - Accent1"/>
+    <tableColumn id="5" xr3:uid="{80928843-3B8E-4E00-9BB2-3CB4E51EAAD3}" name="Area [mm^2] Rounded" dataDxfId="39" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP(Table156[[#This Row],[Area '[mm^2']]], 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{488B557D-7909-401A-A5D7-10BD93B08E9B}" name="Area [L,M,S]" dataDxfId="29" dataCellStyle="20% - Accent1">
+    <tableColumn id="21" xr3:uid="{488B557D-7909-401A-A5D7-10BD93B08E9B}" name="Area [L,M,S]" dataDxfId="38" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Area '[mm^2'] Rounded]]&gt;$AE$53, "L", (IF(Table156[[#This Row],[Area '[mm^2'] Rounded]]&gt;$AE$55, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{803E9B32-8041-46B9-BF42-48214DC67C26}" name="Loading: mg/A [N/m^2]" dataDxfId="41" dataCellStyle="20% - Accent1">
+    <tableColumn id="15" xr3:uid="{803E9B32-8041-46B9-BF42-48214DC67C26}" name="Loading: mg/A [N/m^2]" dataDxfId="37" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>(Table156[[#This Row],[Mass '[g']]]*0.001*9.81)/(Table156[[#This Row],[Area '[mm^2']]]*0.000001)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{423BB4F9-DA2A-4A71-8D56-2F0CE10C71EB}" name="Loading [N/m^2] Rounded" dataDxfId="28" dataCellStyle="20% - Accent1">
+    <tableColumn id="22" xr3:uid="{423BB4F9-DA2A-4A71-8D56-2F0CE10C71EB}" name="Loading [N/m^2] Rounded" dataDxfId="36" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP(Table156[[#This Row],[Loading: mg/A '[N/m^2']]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{08CDF66C-CB66-4E96-945D-B834C0B6FBA2}" name="Loading [L,M,S]" dataDxfId="27" dataCellStyle="20% - Accent1">
+    <tableColumn id="18" xr3:uid="{08CDF66C-CB66-4E96-945D-B834C0B6FBA2}" name="Loading [L,M,S]" dataDxfId="35" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Loading '[N/m^2'] Rounded]]&gt;$AE$37, "L", (IF(Table156[[#This Row],[Loading '[N/m^2'] Rounded]]&gt;$AE$39, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{15862C6A-3975-48AF-ACC0-1ABA3ABD7B75}" name="Span: b [mm]" dataDxfId="40" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="23" xr3:uid="{85241F74-09F8-4D8C-8406-1D0565634FC9}" name="Span: b [mm] Rounded" dataDxfId="26" dataCellStyle="20% - Accent1">
+    <tableColumn id="6" xr3:uid="{15862C6A-3975-48AF-ACC0-1ABA3ABD7B75}" name="Span: b [mm]" dataDxfId="34" dataCellStyle="20% - Accent1"/>
+    <tableColumn id="23" xr3:uid="{85241F74-09F8-4D8C-8406-1D0565634FC9}" name="Span: b [mm] Rounded" dataDxfId="33" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP(Table156[[#This Row],[Span: b '[mm']]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8717B2E8-88BB-4EED-9328-0373DB83A24C}" name="Span [L,M,S]" dataDxfId="24" dataCellStyle="20% - Accent1">
+    <tableColumn id="19" xr3:uid="{8717B2E8-88BB-4EED-9328-0373DB83A24C}" name="Span [L,M,S]" dataDxfId="32" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Span: b '[mm'] Rounded]]&gt;63, "L", (IF(Table156[[#This Row],[Span: b '[mm'] Rounded]]&gt;58, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A2EF55C7-D74D-4B1F-A4BF-04AFD6EE7EF8}" name="Chord: c [mm]" dataDxfId="39" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="24" xr3:uid="{B90185AC-7252-4A87-93C3-28C79AA0AB91}" name="Chord: c [mm] Rounded" dataDxfId="25" dataCellStyle="20% - Accent1">
+    <tableColumn id="7" xr3:uid="{A2EF55C7-D74D-4B1F-A4BF-04AFD6EE7EF8}" name="Chord: c [mm]" dataDxfId="31" dataCellStyle="20% - Accent1"/>
+    <tableColumn id="24" xr3:uid="{B90185AC-7252-4A87-93C3-28C79AA0AB91}" name="Chord: c [mm] Rounded" dataDxfId="30" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP(Table156[[#This Row],[Chord: c '[mm']]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{19F30A62-86CD-4090-9FC5-8ABB2CFA47B0}" name="Chord [L,M,S]" dataDxfId="23" dataCellStyle="20% - Accent1">
+    <tableColumn id="20" xr3:uid="{19F30A62-86CD-4090-9FC5-8ABB2CFA47B0}" name="Chord [L,M,S]" dataDxfId="29" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Chord: c '[mm'] Rounded]]&gt;24.5, "L", (IF(Table156[[#This Row],[Chord: c '[mm'] Rounded]]&gt;21, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{08B57848-CF58-4831-B529-4B940D648C81}" name="Aspect Ratio = b^2/A" dataDxfId="38" dataCellStyle="20% - Accent1">
+    <tableColumn id="9" xr3:uid="{08B57848-CF58-4831-B529-4B940D648C81}" name="Aspect Ratio = b^2/A" dataDxfId="28" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>(K4^2)/E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{046C195E-CF11-4B31-94E7-9E5D67044409}" name="Aspect Ratio = b^2/A Rounded" dataDxfId="22" dataCellStyle="20% - Accent1">
+    <tableColumn id="25" xr3:uid="{046C195E-CF11-4B31-94E7-9E5D67044409}" name="Aspect Ratio = b^2/A Rounded" dataDxfId="27" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP(Table156[[#This Row],[Aspect Ratio = b^2/A]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{667800F5-CAB8-4E53-A0D2-F1E4892A4888}" name="Aspect Ratio[L,M,S]" dataDxfId="21" dataCellStyle="20% - Accent1">
+    <tableColumn id="8" xr3:uid="{667800F5-CAB8-4E53-A0D2-F1E4892A4888}" name="Aspect Ratio[L,M,S]" dataDxfId="26" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Aspect Ratio = b^2/A Rounded]]&gt;$AE$21, "L", (IF(Table156[[#This Row],[Aspect Ratio = b^2/A Rounded]]&gt;$AE$23, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{96D39549-A53E-409A-A985-AF21C6FD140C}" name="Transition Time: t [s]" dataDxfId="37" dataCellStyle="20% - Accent3"/>
-    <tableColumn id="16" xr3:uid="{1E13852D-315C-4703-88AB-A4FF2A94CC9C}" name="Transition Time Descriptor: [Slow, Average, Fast]" dataDxfId="36" dataCellStyle="20% - Accent3">
+    <tableColumn id="11" xr3:uid="{96D39549-A53E-409A-A985-AF21C6FD140C}" name="Transition Time: t [s]" dataDxfId="25" dataCellStyle="20% - Accent3"/>
+    <tableColumn id="16" xr3:uid="{1E13852D-315C-4703-88AB-A4FF2A94CC9C}" name="Transition Time Descriptor: [Slow, Average, Fast]" dataDxfId="24" dataCellStyle="20% - Accent3">
       <calculatedColumnFormula>IF(Table156[[#This Row],[Transition Time: t '[s']]]&gt;$AE$5, "SLOW", (IF(Table156[[#This Row],[Transition Time: t '[s']]]&gt;$AE$7, "AVERAGE", "FAST")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{1464CC48-6A34-4E88-9E75-70DD3FA149B7}" name="1" dataDxfId="35" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="13" xr3:uid="{FA24F7E5-53D2-4912-A65F-7044CD6213CA}" name="2" dataDxfId="34" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="14" xr3:uid="{10A0C0C4-3FE9-4D0B-8D57-9ED26B8333FC}" name="3" dataDxfId="33" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="12" xr3:uid="{1464CC48-6A34-4E88-9E75-70DD3FA149B7}" name="1" dataDxfId="23" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="13" xr3:uid="{FA24F7E5-53D2-4912-A65F-7044CD6213CA}" name="2" dataDxfId="22" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="14" xr3:uid="{10A0C0C4-3FE9-4D0B-8D57-9ED26B8333FC}" name="3" dataDxfId="21" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7608,7 +5246,13 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A5AC6ABD-4DAE-48F0-AFE3-0DD771DD2CAB}" name="Table1567" displayName="Table1567" ref="A3:S87" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowCellStyle="Heading 3" dataCellStyle="20% - Accent5">
-  <autoFilter ref="A3:S87" xr:uid="{E5B61A00-5AF6-2A4A-9778-06EAC2F9166B}"/>
+  <autoFilter ref="A3:S87" xr:uid="{E5B61A00-5AF6-2A4A-9778-06EAC2F9166B}">
+    <filterColumn colId="15">
+      <filters>
+        <filter val="FAST"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:S87">
     <sortCondition ref="B3:B87"/>
   </sortState>
@@ -7640,16 +5284,16 @@
     <tableColumn id="9" xr3:uid="{0360C153-9D20-4787-B5F0-C207DEE37844}" name="Aspect Ratio = b^2/A" dataDxfId="6" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>ROUNDUP((Table1567[[#This Row],[Span: b '[mm']]]^2)/Table1567[[#This Row],[Area '[mm^2']]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{217BF731-A5BF-4977-910D-E50A20EFB45F}" name="Aspect Ratio[L,M,S]" dataDxfId="0" dataCellStyle="20% - Accent1">
+    <tableColumn id="8" xr3:uid="{217BF731-A5BF-4977-910D-E50A20EFB45F}" name="Aspect Ratio[L,M,S]" dataDxfId="5" dataCellStyle="20% - Accent1">
       <calculatedColumnFormula>IF(Table1567[[#This Row],[Aspect Ratio = b^2/A]]&gt;$AH$5, "L", (IF(Table1567[[#This Row],[Aspect Ratio = b^2/A]]&gt;$AH$7, "M", "S")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AFA51A67-18E5-4684-807C-2878F2065737}" name="Transition Time: t [s]" dataDxfId="5" dataCellStyle="20% - Accent3"/>
-    <tableColumn id="16" xr3:uid="{8201CA0D-C85F-4610-8456-33A3C49BC0DC}" name="Transition Time Descriptor: [Slow, Average, Fast]" dataDxfId="4" dataCellStyle="20% - Accent3">
+    <tableColumn id="11" xr3:uid="{AFA51A67-18E5-4684-807C-2878F2065737}" name="Transition Time: t [s]" dataDxfId="4" dataCellStyle="20% - Accent3"/>
+    <tableColumn id="16" xr3:uid="{8201CA0D-C85F-4610-8456-33A3C49BC0DC}" name="Transition Time Descriptor: [Slow, Average, Fast]" dataDxfId="3" dataCellStyle="20% - Accent3">
       <calculatedColumnFormula>IF(Table1567[[#This Row],[Transition Time: t '[s']]]&gt;$Z$5, "SLOW", (IF(Table1567[[#This Row],[Transition Time: t '[s']]]&gt;$Z$7, "AVERAGE", "FAST")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5967FC1A-A724-4C8F-98B0-A43CA7E8288D}" name="1" dataDxfId="3" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="13" xr3:uid="{4D5CC357-0393-4B28-B2E4-00A074AC3EFD}" name="2" dataDxfId="2" dataCellStyle="20% - Accent5"/>
-    <tableColumn id="14" xr3:uid="{3CFCF80A-282E-4614-BC43-A6237FE1CDF9}" name="3" dataDxfId="1" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="12" xr3:uid="{5967FC1A-A724-4C8F-98B0-A43CA7E8288D}" name="1" dataDxfId="2" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="13" xr3:uid="{4D5CC357-0393-4B28-B2E4-00A074AC3EFD}" name="2" dataDxfId="1" dataCellStyle="20% - Accent5"/>
+    <tableColumn id="14" xr3:uid="{3CFCF80A-282E-4614-BC43-A6237FE1CDF9}" name="3" dataDxfId="0" dataCellStyle="20% - Accent5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7974,8 +5618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE7E1BF-C345-41B2-A1E7-99751C84928F}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14002,7 +11646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68552E6A-184C-40A9-9BC4-F9CCBA2B8C3E}">
   <dimension ref="A1:AM86"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -20299,10 +17943,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6268479-2E0E-4ACF-85FE-CD176DDA1192}">
-  <dimension ref="A1:AQ87"/>
+  <dimension ref="A1:AQ113"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20313,7 +17957,7 @@
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
@@ -26157,7 +23801,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>70</v>
       </c>
@@ -26320,6 +23964,10 @@
       <c r="V67" s="9"/>
       <c r="W67" s="9"/>
       <c r="X67" s="9"/>
+      <c r="Z67" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA67" s="24"/>
     </row>
     <row r="68" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -26402,6 +24050,8 @@
       <c r="V68" s="9"/>
       <c r="W68" s="9"/>
       <c r="X68" s="9"/>
+      <c r="Z68" s="22"/>
+      <c r="AA68" s="22"/>
     </row>
     <row r="69" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -26484,6 +24134,12 @@
       <c r="V69" s="9"/>
       <c r="W69" s="9"/>
       <c r="X69" s="9"/>
+      <c r="Z69" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA69" s="22">
+        <v>0.45952380952380945</v>
+      </c>
     </row>
     <row r="70" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -26566,6 +24222,12 @@
       <c r="V70" s="9"/>
       <c r="W70" s="9"/>
       <c r="X70" s="9"/>
+      <c r="Z70" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA70" s="22">
+        <v>1.4283323571232524E-2</v>
+      </c>
     </row>
     <row r="71" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -26654,6 +24316,12 @@
       <c r="X71" s="9">
         <v>0.435</v>
       </c>
+      <c r="Z71" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA71" s="22">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="72" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -26736,6 +24404,12 @@
       <c r="V72" s="9"/>
       <c r="W72" s="9"/>
       <c r="X72" s="9"/>
+      <c r="Z72" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA72" s="22">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="73" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -26818,6 +24492,12 @@
       <c r="V73" s="9"/>
       <c r="W73" s="9"/>
       <c r="X73" s="9"/>
+      <c r="Z73" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA73" s="22">
+        <v>0.13090882288144001</v>
+      </c>
     </row>
     <row r="74" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -26900,6 +24580,12 @@
       <c r="V74" s="9"/>
       <c r="W74" s="9"/>
       <c r="X74" s="9"/>
+      <c r="Z74" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA74" s="22">
+        <v>1.7137119908204233E-2</v>
+      </c>
     </row>
     <row r="75" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -26982,6 +24668,12 @@
       <c r="V75" s="9"/>
       <c r="W75" s="9"/>
       <c r="X75" s="9"/>
+      <c r="Z75" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA75" s="22">
+        <v>1.1583715789136306E-3</v>
+      </c>
     </row>
     <row r="76" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -27064,6 +24756,12 @@
       <c r="V76" s="9"/>
       <c r="W76" s="9"/>
       <c r="X76" s="9"/>
+      <c r="Z76" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA76" s="22">
+        <v>6.7602249818898591E-2</v>
+      </c>
     </row>
     <row r="77" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -27146,6 +24844,12 @@
       <c r="V77" s="9"/>
       <c r="W77" s="9"/>
       <c r="X77" s="9"/>
+      <c r="Z77" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA77" s="22">
+        <v>0.70000000000000007</v>
+      </c>
     </row>
     <row r="78" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -27228,6 +24932,12 @@
       <c r="V78" s="9"/>
       <c r="W78" s="9"/>
       <c r="X78" s="9"/>
+      <c r="Z78" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA78" s="22">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="79" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -27316,6 +25026,12 @@
       <c r="X79" s="9">
         <v>0.33700000000000002</v>
       </c>
+      <c r="Z79" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA79" s="22">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="80" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -27398,8 +25114,14 @@
       <c r="V80" s="9"/>
       <c r="W80" s="9"/>
       <c r="X80" s="9"/>
-    </row>
-    <row r="81" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z80" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA80" s="22">
+        <v>38.599999999999994</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>88</v>
       </c>
@@ -27480,8 +25202,14 @@
       <c r="V81" s="9"/>
       <c r="W81" s="9"/>
       <c r="X81" s="9"/>
-    </row>
-    <row r="82" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z81" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA81" s="23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>89</v>
       </c>
@@ -27563,7 +25291,7 @@
       <c r="W82" s="9"/>
       <c r="X82" s="9"/>
     </row>
-    <row r="83" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>90</v>
       </c>
@@ -27644,8 +25372,12 @@
       <c r="V83" s="9"/>
       <c r="W83" s="9"/>
       <c r="X83" s="9"/>
-    </row>
-    <row r="84" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z83" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA83" s="24"/>
+    </row>
+    <row r="84" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>91</v>
       </c>
@@ -27726,8 +25458,10 @@
       <c r="V84" s="9"/>
       <c r="W84" s="9"/>
       <c r="X84" s="9"/>
-    </row>
-    <row r="85" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z84" s="22"/>
+      <c r="AA84" s="22"/>
+    </row>
+    <row r="85" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>93</v>
       </c>
@@ -27808,8 +25542,14 @@
       <c r="V85" s="9"/>
       <c r="W85" s="9"/>
       <c r="X85" s="9"/>
-    </row>
-    <row r="86" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z85" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA85" s="22">
+        <v>60.095833333333381</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>94</v>
       </c>
@@ -27890,8 +25630,14 @@
       <c r="V86" s="9"/>
       <c r="W86" s="9"/>
       <c r="X86" s="9"/>
-    </row>
-    <row r="87" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z86" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA86" s="22">
+        <v>0.6749370512780638</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>96</v>
       </c>
@@ -27972,15 +25718,216 @@
       <c r="V87" s="9"/>
       <c r="W87" s="9"/>
       <c r="X87" s="9"/>
+      <c r="Z87" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA87" s="22">
+        <v>60.56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z88" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA88" s="22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z89" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA89" s="22">
+        <v>6.1859002536240366</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z90" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA90" s="22">
+        <v>38.265361947785919</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z91" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA91" s="22">
+        <v>-0.51270339726348935</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z92" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA92" s="22">
+        <v>-4.9297075627241761E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z93" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA93" s="22">
+        <v>27.810000000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z94" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA94" s="22">
+        <v>45.11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z95" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA95" s="22">
+        <v>72.92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z96" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA96" s="22">
+        <v>5048.0500000000038</v>
+      </c>
+    </row>
+    <row r="97" spans="26:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z97" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA97" s="23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="26:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z99" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA99" s="24"/>
+    </row>
+    <row r="100" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z100" s="22"/>
+      <c r="AA100" s="22"/>
+    </row>
+    <row r="101" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z101" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA101" s="22">
+        <v>23.028690476190473</v>
+      </c>
+    </row>
+    <row r="102" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z102" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA102" s="22">
+        <v>0.29821128538886027</v>
+      </c>
+    </row>
+    <row r="103" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z103" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA103" s="22">
+        <v>22.68</v>
+      </c>
+    </row>
+    <row r="104" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z104" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA104" s="22">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="105" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z105" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA105" s="22">
+        <v>2.7331515767690613</v>
+      </c>
+    </row>
+    <row r="106" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z106" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA106" s="22">
+        <v>7.470117541595207</v>
+      </c>
+    </row>
+    <row r="107" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z107" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA107" s="22">
+        <v>-0.66958901692884121</v>
+      </c>
+    </row>
+    <row r="108" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z108" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA108" s="22">
+        <v>0.28132139491345393</v>
+      </c>
+    </row>
+    <row r="109" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z109" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA109" s="22">
+        <v>11.579999999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z110" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA110" s="22">
+        <v>17.720000000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z111" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA111" s="22">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="112" spans="26:27" x14ac:dyDescent="0.25">
+      <c r="Z112" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA112" s="22">
+        <v>1934.4099999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="26:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z113" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA113" s="23">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Z51:AA51"/>
     <mergeCell ref="C1:S1"/>
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="Z51:AA51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27994,8 +25941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95565C6-F0A7-4F1E-8FE2-588B19A5EB00}">
   <dimension ref="A1:AI87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28131,20 +26078,20 @@
       <c r="S3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="V3" s="25"/>
-      <c r="AC3" s="24" t="s">
+      <c r="V3" s="21"/>
+      <c r="AC3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" s="24"/>
+      <c r="AD3" s="15"/>
       <c r="AF3" s="18"/>
       <c r="AG3" s="18"/>
       <c r="AH3" s="18"/>
       <c r="AI3" s="18"/>
     </row>
-    <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -28205,16 +26152,12 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
       <c r="AF4" s="18"/>
       <c r="AG4" s="18"/>
       <c r="AH4" s="18"/>
       <c r="AI4" s="18"/>
     </row>
-    <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -28275,10 +26218,10 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="U5" s="22" t="s">
+      <c r="U5" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="22">
+      <c r="V5">
         <v>0.47192261904761912</v>
       </c>
       <c r="X5" s="18" t="s">
@@ -28292,10 +26235,10 @@
         <v>0.52327584269132077</v>
       </c>
       <c r="AA5" s="18"/>
-      <c r="AC5" s="22" t="s">
+      <c r="AC5" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="22">
+      <c r="AD5">
         <v>3.487738095238095</v>
       </c>
       <c r="AF5" s="18" t="s">
@@ -28377,10 +26320,10 @@
       <c r="S6" s="9">
         <v>0.36099999999999999</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="U6" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="22">
+      <c r="V6">
         <v>5.6030960601728226E-3</v>
       </c>
       <c r="X6" s="18" t="s">
@@ -28397,10 +26340,10 @@
         <f>Z5</f>
         <v>0.52327584269132077</v>
       </c>
-      <c r="AC6" s="22" t="s">
+      <c r="AC6" t="s">
         <v>21</v>
       </c>
-      <c r="AD6" s="22">
+      <c r="AD6">
         <v>3.9777187518562018E-2</v>
       </c>
       <c r="AF6" s="18" t="s">
@@ -28418,7 +26361,7 @@
         <v>3.852302040710621</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -28479,10 +26422,10 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="U7" s="22" t="s">
+      <c r="U7" t="s">
         <v>22</v>
       </c>
-      <c r="V7" s="22">
+      <c r="V7">
         <v>0.47</v>
       </c>
       <c r="X7" s="18" t="s">
@@ -28496,10 +26439,10 @@
         <v>0.42056939540391752</v>
       </c>
       <c r="AA7" s="18"/>
-      <c r="AC7" s="22" t="s">
+      <c r="AC7" t="s">
         <v>22</v>
       </c>
-      <c r="AD7" s="22">
+      <c r="AD7">
         <v>3.46</v>
       </c>
       <c r="AF7" s="18" t="s">
@@ -28514,7 +26457,7 @@
       </c>
       <c r="AI7" s="18"/>
     </row>
-    <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -28575,24 +26518,24 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="U8" s="22" t="s">
+      <c r="U8" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="22">
+      <c r="V8">
         <v>0.47</v>
       </c>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
       <c r="AA8" s="18"/>
-      <c r="AC8" s="22" t="s">
+      <c r="AC8" t="s">
         <v>23</v>
       </c>
-      <c r="AD8" s="22">
+      <c r="AD8">
         <v>3.6599999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -28653,20 +26596,20 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="U9" s="22" t="s">
+      <c r="U9" t="s">
         <v>24</v>
       </c>
-      <c r="V9" s="22">
+      <c r="V9">
         <v>5.1353223643701602E-2</v>
       </c>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
-      <c r="AC9" s="22" t="s">
+      <c r="AC9" t="s">
         <v>24</v>
       </c>
-      <c r="AD9" s="22">
+      <c r="AD9">
         <v>0.36456394547252619</v>
       </c>
     </row>
@@ -28731,20 +26674,20 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="U10" s="22" t="s">
+      <c r="U10" t="s">
         <v>25</v>
       </c>
-      <c r="V10" s="22">
+      <c r="V10">
         <v>2.6371535786000331E-3</v>
       </c>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
-      <c r="AC10" s="22" t="s">
+      <c r="AC10" t="s">
         <v>25</v>
       </c>
-      <c r="AD10" s="22">
+      <c r="AD10">
         <v>0.13290687033849505</v>
       </c>
     </row>
@@ -28815,24 +26758,24 @@
       <c r="S11" s="9">
         <v>0.47799999999999998</v>
       </c>
-      <c r="U11" s="22" t="s">
+      <c r="U11" t="s">
         <v>26</v>
       </c>
-      <c r="V11" s="22">
+      <c r="V11">
         <v>0.946739535687251</v>
       </c>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
       <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
-      <c r="AC11" s="22" t="s">
+      <c r="AC11" t="s">
         <v>26</v>
       </c>
-      <c r="AD11" s="22">
+      <c r="AD11">
         <v>1.9746741143280984</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -28893,24 +26836,24 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
-      <c r="U12" s="22" t="s">
+      <c r="U12" t="s">
         <v>27</v>
       </c>
-      <c r="V12" s="22">
+      <c r="V12">
         <v>0.51006960395610834</v>
       </c>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
       <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
-      <c r="AC12" s="22" t="s">
+      <c r="AC12" t="s">
         <v>27</v>
       </c>
-      <c r="AD12" s="22">
+      <c r="AD12">
         <v>0.78620840872131348</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -28977,24 +26920,24 @@
       <c r="S13" s="9">
         <v>0.436</v>
       </c>
-      <c r="U13" s="22" t="s">
+      <c r="U13" t="s">
         <v>28</v>
       </c>
-      <c r="V13" s="22">
+      <c r="V13">
         <v>0.26</v>
       </c>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
-      <c r="AC13" s="22" t="s">
+      <c r="AC13" t="s">
         <v>28</v>
       </c>
-      <c r="AD13" s="22">
+      <c r="AD13">
         <v>2.0799999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -29055,24 +26998,24 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
-      <c r="U14" s="22" t="s">
+      <c r="U14" t="s">
         <v>29</v>
       </c>
-      <c r="V14" s="22">
+      <c r="V14">
         <v>0.36399999999999999</v>
       </c>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
-      <c r="AC14" s="22" t="s">
+      <c r="AC14" t="s">
         <v>29</v>
       </c>
-      <c r="AD14" s="22">
+      <c r="AD14">
         <v>2.73</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -29133,24 +27076,24 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="U15" s="22" t="s">
+      <c r="U15" t="s">
         <v>30</v>
       </c>
-      <c r="V15" s="22">
+      <c r="V15">
         <v>0.624</v>
       </c>
       <c r="X15" s="18"/>
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
-      <c r="AC15" s="22" t="s">
+      <c r="AC15" t="s">
         <v>30</v>
       </c>
-      <c r="AD15" s="22">
+      <c r="AD15">
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -29211,24 +27154,24 @@
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="U16" s="22" t="s">
+      <c r="U16" t="s">
         <v>31</v>
       </c>
-      <c r="V16" s="22">
+      <c r="V16">
         <v>39.641500000000008</v>
       </c>
       <c r="X16" s="18"/>
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
-      <c r="AC16" s="22" t="s">
+      <c r="AC16" t="s">
         <v>31</v>
       </c>
-      <c r="AD16" s="22">
+      <c r="AD16">
         <v>292.96999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -29289,24 +27232,24 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
-      <c r="U17" s="23" t="s">
+      <c r="U17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="V17" s="23">
+      <c r="V17" s="12">
         <v>84</v>
       </c>
       <c r="X17" s="18"/>
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
       <c r="AA17" s="18"/>
-      <c r="AC17" s="23" t="s">
+      <c r="AC17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AD17" s="23">
+      <c r="AD17" s="12">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -29372,7 +27315,7 @@
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
     </row>
-    <row r="19" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -29434,7 +27377,7 @@
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -29496,7 +27439,7 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
     </row>
-    <row r="21" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -29564,7 +27507,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -29632,7 +27575,7 @@
         <v>0.42199999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -29694,7 +27637,7 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -29818,7 +27761,7 @@
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -29880,7 +27823,7 @@
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -30010,7 +27953,7 @@
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
     </row>
-    <row r="29" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -30134,7 +28077,7 @@
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
     </row>
-    <row r="31" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -30196,7 +28139,7 @@
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
     </row>
-    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -30258,7 +28201,7 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
     </row>
-    <row r="33" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -30320,7 +28263,7 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
     </row>
-    <row r="34" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -30382,7 +28325,7 @@
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
     </row>
-    <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -30448,7 +28391,7 @@
       </c>
       <c r="V35" s="21"/>
     </row>
-    <row r="36" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -30510,7 +28453,7 @@
       <c r="R36" s="9"/>
       <c r="S36" s="9"/>
     </row>
-    <row r="37" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>38</v>
       </c>
@@ -30589,7 +28532,7 @@
       </c>
       <c r="AA37" s="18"/>
     </row>
-    <row r="38" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39</v>
       </c>
@@ -30671,7 +28614,7 @@
         <v>5.4884356908883403</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>40</v>
       </c>
@@ -30750,7 +28693,7 @@
       </c>
       <c r="AA39" s="18"/>
     </row>
-    <row r="40" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42</v>
       </c>
@@ -30818,7 +28761,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43</v>
       </c>
@@ -30960,7 +28903,7 @@
         <v>1.3451930459303552</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>46</v>
       </c>
@@ -31028,7 +28971,7 @@
         <v>0.8473174712085485</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>47</v>
       </c>
@@ -31096,7 +29039,7 @@
         <v>0.57662052144943787</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>49</v>
       </c>
@@ -31232,7 +29175,7 @@
         <v>1.3610558365817524</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>51</v>
       </c>
@@ -31300,7 +29243,7 @@
         <v>7.5547302540519432</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>52</v>
       </c>
@@ -31368,7 +29311,7 @@
         <v>363.60333369274366</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>53</v>
       </c>
@@ -31436,7 +29379,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>54</v>
       </c>
@@ -31498,7 +29441,7 @@
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
     </row>
-    <row r="51" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>55</v>
       </c>
@@ -31632,7 +29575,7 @@
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
     </row>
-    <row r="53" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>57</v>
       </c>
@@ -31711,7 +29654,7 @@
       </c>
       <c r="AA53" s="18"/>
     </row>
-    <row r="54" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>58</v>
       </c>
@@ -31793,7 +29736,7 @@
         <v>1258.3630672908646</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>59</v>
       </c>
@@ -31872,7 +29815,7 @@
       </c>
       <c r="AA55" s="18"/>
     </row>
-    <row r="56" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>60</v>
       </c>
@@ -31940,7 +29883,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>61</v>
       </c>
@@ -32008,7 +29951,7 @@
         <v>207.59431861586464</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>62</v>
       </c>
@@ -32082,7 +30025,7 @@
         <v>43095.401121585128</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>63</v>
       </c>
@@ -32150,7 +30093,7 @@
         <v>8.542744870018959E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>64</v>
       </c>
@@ -32292,7 +30235,7 @@
         <v>939.96753489999992</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>66</v>
       </c>
@@ -32360,7 +30303,7 @@
         <v>629.96152910000001</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>67</v>
       </c>
@@ -32428,7 +30371,7 @@
         <v>1569.9290639999999</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>68</v>
       </c>
@@ -32496,7 +30439,7 @@
         <v>88264.574888699994</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>69</v>
       </c>
@@ -32564,7 +30507,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>70</v>
       </c>
@@ -32626,7 +30569,7 @@
       <c r="R66" s="9"/>
       <c r="S66" s="9"/>
     </row>
-    <row r="67" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>71</v>
       </c>
@@ -32688,7 +30631,7 @@
       <c r="R67" s="9"/>
       <c r="S67" s="9"/>
     </row>
-    <row r="68" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>72</v>
       </c>
@@ -32750,7 +30693,7 @@
       <c r="R68" s="9"/>
       <c r="S68" s="9"/>
     </row>
-    <row r="69" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>74</v>
       </c>
@@ -32812,7 +30755,7 @@
       <c r="R69" s="9"/>
       <c r="S69" s="9"/>
     </row>
-    <row r="70" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>75</v>
       </c>
@@ -32874,7 +30817,7 @@
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
     </row>
-    <row r="71" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>76</v>
       </c>
@@ -32942,7 +30885,7 @@
         <v>0.435</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>77</v>
       </c>
@@ -33004,7 +30947,7 @@
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
     </row>
-    <row r="73" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>78</v>
       </c>
@@ -33066,7 +31009,7 @@
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
     </row>
-    <row r="74" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>79</v>
       </c>
@@ -33128,7 +31071,7 @@
       <c r="R74" s="9"/>
       <c r="S74" s="9"/>
     </row>
-    <row r="75" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>81</v>
       </c>
@@ -33190,7 +31133,7 @@
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
     </row>
-    <row r="76" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>82</v>
       </c>
@@ -33252,7 +31195,7 @@
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
     </row>
-    <row r="77" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>83</v>
       </c>
@@ -33314,7 +31257,7 @@
       <c r="R77" s="9"/>
       <c r="S77" s="9"/>
     </row>
-    <row r="78" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>84</v>
       </c>
@@ -33444,7 +31387,7 @@
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>87</v>
       </c>
@@ -33506,7 +31449,7 @@
       <c r="R80" s="9"/>
       <c r="S80" s="9"/>
     </row>
-    <row r="81" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>88</v>
       </c>
@@ -33568,7 +31511,7 @@
       <c r="R81" s="9"/>
       <c r="S81" s="9"/>
     </row>
-    <row r="82" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>89</v>
       </c>
@@ -33630,7 +31573,7 @@
       <c r="R82" s="9"/>
       <c r="S82" s="9"/>
     </row>
-    <row r="83" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>90</v>
       </c>
@@ -33692,7 +31635,7 @@
       <c r="R83" s="9"/>
       <c r="S83" s="9"/>
     </row>
-    <row r="84" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>91</v>
       </c>
@@ -33754,7 +31697,7 @@
       <c r="R84" s="9"/>
       <c r="S84" s="9"/>
     </row>
-    <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>93</v>
       </c>
@@ -33816,7 +31759,7 @@
       <c r="R85" s="9"/>
       <c r="S85" s="9"/>
     </row>
-    <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>94</v>
       </c>
@@ -33878,7 +31821,7 @@
       <c r="R86" s="9"/>
       <c r="S86" s="9"/>
     </row>
-    <row r="87" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>96</v>
       </c>

</xml_diff>